<commit_message>
added the fail test for user email or password failed
</commit_message>
<xml_diff>
--- a/src/main/resources/output.xlsx
+++ b/src/main/resources/output.xlsx
@@ -6,7 +6,7 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Comprar test excel" r:id="rId3" sheetId="1"/>
+    <sheet name="Comprar test excel fail" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
@@ -20,13 +20,13 @@
     <t>In Cart</t>
   </si>
   <si>
-    <t>Samsung Galaxy Tab 10.1</t>
+    <t>fail</t>
+  </si>
+  <si>
+    <t>Not In Cart</t>
   </si>
   <si>
     <t>HTC Touch HD</t>
-  </si>
-  <si>
-    <t>Nikon D300</t>
   </si>
   <si>
     <t>iPhone</t>
@@ -93,12 +93,12 @@
         <v>2</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s" s="0">
         <v>1</v>
@@ -106,10 +106,10 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">

</xml_diff>